<commit_message>
Fixed more schematic errors
</commit_message>
<xml_diff>
--- a/Hardware/Pinto/Project Outputs for Pinto/Pinto_BOM.xlsx
+++ b/Hardware/Pinto/Project Outputs for Pinto/Pinto_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bscha\Desktop\Pinto\Hardware\Pinto\Project Outputs for Pinto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98715FA-46C5-4E69-872C-7B8DD4DD34A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E665600-CBD8-4265-A9A6-C12AC6900C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E798C1C2-2D61-460F-8336-4B3FD7EFD4F0}"/>
+    <workbookView xWindow="8460" yWindow="4245" windowWidth="28800" windowHeight="15345" xr2:uid="{E798C1C2-2D61-460F-8336-4B3FD7EFD4F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Pinto_BOM" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="125">
   <si>
     <t>Comment</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>Capacitor 12pF +/-10% 50V 0402</t>
-  </si>
-  <si>
     <t>Chip Capacitor, 12pF +/-10%, 50V, 0402, Thickness 0.33 mm</t>
   </si>
   <si>
@@ -113,12 +110,6 @@
     <t>CMP-001-00074-3</t>
   </si>
   <si>
-    <t>Capacitor 0.1 uF +/- 5% 16 V 0402</t>
-  </si>
-  <si>
-    <t>Chip Capacitor, 0.1 uF, +/- 5%, 16 V, 0402 (1005 Metric)</t>
-  </si>
-  <si>
     <t>C11, C12</t>
   </si>
   <si>
@@ -245,15 +236,9 @@
     <t>CMP-0434-00001-1</t>
   </si>
   <si>
-    <t>10KR2F</t>
-  </si>
-  <si>
     <t>10K 0.063W 1% 0402 (1005 Metric)  SMD</t>
   </si>
   <si>
-    <t>R1</t>
-  </si>
-  <si>
     <t>RESC0402(1005)_L</t>
   </si>
   <si>
@@ -266,9 +251,6 @@
     <t>Jumper 0402 (1005 Metric)</t>
   </si>
   <si>
-    <t>R2, R3, R4, R5</t>
-  </si>
-  <si>
     <t>CMP-009-00062-2</t>
   </si>
   <si>
@@ -359,9 +341,6 @@
     <t>Mouser Part #</t>
   </si>
   <si>
-    <t>581-04025A120F4T2A</t>
-  </si>
-  <si>
     <t>581-0402YD105KAT2A</t>
   </si>
   <si>
@@ -386,9 +365,6 @@
     <t>512-2N7002</t>
   </si>
   <si>
-    <t>279-CRG0402F10K</t>
-  </si>
-  <si>
     <t>673-BSPQ000603042N2B</t>
   </si>
   <si>
@@ -404,10 +380,40 @@
     <t>485-1655</t>
   </si>
   <si>
-    <t>10 PACK</t>
-  </si>
-  <si>
     <t>611-PTS810SJM250SMTR</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Capacitor 8pF +/-10% 50V 0402</t>
+  </si>
+  <si>
+    <t>581-04023A8R0CAT2A</t>
+  </si>
+  <si>
+    <t>Capacitor 3,3 uF +/- 5% 16 V 0402</t>
+  </si>
+  <si>
+    <t>80-CBR04C339B5GAUTO</t>
+  </si>
+  <si>
+    <t>Chip Capacitor, 3.3 uF, +/- 5%, 16 V, 0402 (1005 Metric)</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R1,R3, R4, R5</t>
+  </si>
+  <si>
+    <t>5k1</t>
+  </si>
+  <si>
+    <t>603-RT0402FRE075K1L</t>
+  </si>
+  <si>
+    <t>10 PACK (ONLY NEED 1)</t>
   </si>
 </sst>
 </file>
@@ -449,7 +455,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -472,11 +478,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -484,6 +501,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -801,7 +819,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,435 +847,445 @@
         <v>5</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="F2" s="1">
         <v>2</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>106</v>
+        <v>116</v>
+      </c>
+      <c r="K2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="F3" s="1">
         <v>6</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="F4" s="1">
         <v>5</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="K4" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="F6" s="1">
         <v>2</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="K6" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="F8" s="1">
         <v>1</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="F11" s="1">
         <v>1</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="F12" s="1">
         <v>1</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="E13" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F13" s="1">
         <v>2</v>
       </c>
+      <c r="H13" s="6" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="E14" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="H14" s="6" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="F15" s="1">
         <v>1</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>68</v>
+        <v>122</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>70</v>
+        <v>121</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F16" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>120</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F17" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F18" s="1">
         <v>4</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F19" s="1">
         <v>2</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="F20" s="1">
         <v>1</v>
@@ -1265,74 +1293,74 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="F21" s="1">
         <v>1</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="K21" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="F22" s="1">
         <v>1</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F23" s="1">
         <v>1</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>